<commit_message>
Dots on the i
Added links to several pages
</commit_message>
<xml_diff>
--- a/Documentatie project/Logboek_John_Ronald.xlsx
+++ b/Documentatie project/Logboek_John_Ronald.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="81">
   <si>
     <t>Wie</t>
   </si>
@@ -258,6 +258,15 @@
   </si>
   <si>
     <t>Verder aan werken (alle pagina's maken)</t>
+  </si>
+  <si>
+    <t>80 min</t>
+  </si>
+  <si>
+    <t>V2.0 bijwerken, pagina's toegevoegd</t>
+  </si>
+  <si>
+    <t>gecontroleerd door John</t>
   </si>
 </sst>
 </file>
@@ -606,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1104,6 +1113,23 @@
         <v>77</v>
       </c>
     </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
css uit html gehaald
</commit_message>
<xml_diff>
--- a/Documentatie project/Logboek_John_Ronald.xlsx
+++ b/Documentatie project/Logboek_John_Ronald.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="99">
   <si>
     <t>Wie</t>
   </si>
@@ -306,6 +306,21 @@
   </si>
   <si>
     <t>Website online gezet + uitzoeken hoe</t>
+  </si>
+  <si>
+    <t>Login form op iedere pagina zetten</t>
+  </si>
+  <si>
+    <t>120min</t>
+  </si>
+  <si>
+    <t>Reflectie geschreven (individueel)</t>
+  </si>
+  <si>
+    <t>Optimalisatieplan aangemaakt</t>
+  </si>
+  <si>
+    <t>30min</t>
   </si>
 </sst>
 </file>
@@ -654,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1288,6 +1303,45 @@
         <v>46</v>
       </c>
     </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>42387</v>
+      </c>
+      <c r="B34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>42388</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>42389</v>
+      </c>
+      <c r="B36" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>